<commit_message>
Fix issue with columns redundance
</commit_message>
<xml_diff>
--- a/diff/xlsx/fruits_diff.xlsx
+++ b/diff/xlsx/fruits_diff.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,15 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>FIELD</t>
+          <t>fruits_df1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>fruits_df2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>LOCATION</t>
         </is>
@@ -453,6 +458,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>apple</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>In both DataFrames</t>
         </is>
       </c>
@@ -465,6 +475,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>banana</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>In both DataFrames</t>
         </is>
       </c>
@@ -477,17 +492,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>cherry</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>In both DataFrames</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
         <is>
           <t>grape</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>In fruits_df2 only</t>
         </is>
@@ -499,7 +520,8 @@
           <t>kiwi</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
         <is>
           <t>In fruits_df1 only</t>
         </is>
@@ -511,7 +533,8 @@
           <t>mango</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
         <is>
           <t>In fruits_df1 only</t>
         </is>
@@ -523,31 +546,34 @@
           <t>peach</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
         <is>
           <t>In fruits_df1 only</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
         <is>
           <t>pear</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>In fruits_df2 only</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
         <is>
           <t>watermelon</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>In fruits_df2 only</t>
         </is>

</xml_diff>